<commit_message>
minor updates to analysis
</commit_message>
<xml_diff>
--- a/analysis/childcare anticipation.xlsx
+++ b/analysis/childcare anticipation.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693C6986-AD98-4FB2-B68F-DD1AE865F824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593D0F0F-A5D8-4633-85DB-BCA1E38AF24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF257537-61BE-417F-A610-2BEACBAD6A2E}"/>
   </bookViews>
   <sheets>
-    <sheet name="coarse" sheetId="7" r:id="rId1"/>
-    <sheet name="zero" sheetId="2" r:id="rId2"/>
-    <sheet name="naive" sheetId="4" r:id="rId3"/>
-    <sheet name="base" sheetId="1" r:id="rId4"/>
-    <sheet name="naive - zero" sheetId="6" r:id="rId5"/>
-    <sheet name="base - naive" sheetId="5" r:id="rId6"/>
-    <sheet name="base - zero" sheetId="3" r:id="rId7"/>
+    <sheet name="zero" sheetId="2" r:id="rId1"/>
+    <sheet name="naive" sheetId="4" r:id="rId2"/>
+    <sheet name="base" sheetId="1" r:id="rId3"/>
+    <sheet name="naive - zero" sheetId="6" r:id="rId4"/>
+    <sheet name="base - naive" sheetId="5" r:id="rId5"/>
+    <sheet name="base - zero" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="30">
   <si>
     <t>age</t>
   </si>
@@ -133,72 +132,6 @@
   <si>
     <t>small effects</t>
   </si>
-  <si>
-    <t>zero</t>
-  </si>
-  <si>
-    <t>emp hours</t>
-  </si>
-  <si>
-    <t>number emp</t>
-  </si>
-  <si>
-    <t>partners</t>
-  </si>
-  <si>
-    <t>care hours</t>
-  </si>
-  <si>
-    <t>child care costs per week</t>
-  </si>
-  <si>
-    <t>formal care expenditure weekly</t>
-  </si>
-  <si>
-    <t>disposable income per month</t>
-  </si>
-  <si>
-    <t>naïve</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>Differences</t>
-  </si>
-  <si>
-    <t>anticipation</t>
-  </si>
-  <si>
-    <t>women under age 37 without children</t>
-  </si>
-  <si>
-    <t>impact</t>
-  </si>
-  <si>
-    <t>with at least one child aged 0 to 4 and no other children</t>
-  </si>
-  <si>
-    <t>with one child aged 0 to 4 and no other children</t>
-  </si>
-  <si>
-    <t>women under age 37 without children no disabled</t>
-  </si>
-  <si>
-    <t>with at least one child aged 0 to 4 and no other children no disabled</t>
-  </si>
-  <si>
-    <t>with at least one child aged 0 to 4 and no other children no disabled no care hours</t>
-  </si>
-  <si>
-    <t>women under age 37 without children no disabled no carers</t>
-  </si>
-  <si>
-    <t>scarring</t>
-  </si>
-  <si>
-    <t>with at least one child aged 15 to 17 and no other children no disabled no care hours</t>
-  </si>
 </sst>
 </file>
 
@@ -213,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,12 +156,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,11 +172,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,2039 +508,842 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9BF38E-B32A-4497-8003-918DB92F7A84}">
-  <dimension ref="A1:R60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8658D477-A0FD-4579-B4B5-2D0B91304A87}">
+  <dimension ref="A2:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>46</v>
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
       </c>
       <c r="Q2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="R2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>17.83944</v>
+      </c>
+      <c r="C3">
+        <v>0.2153149</v>
       </c>
       <c r="D3">
-        <v>23.288450000000001</v>
+        <v>0.16747629999999999</v>
       </c>
       <c r="E3">
-        <v>22.727239999999998</v>
+        <v>0.61720870000000005</v>
       </c>
       <c r="F3">
-        <v>22.375350000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <f>E3-D3</f>
-        <v>-0.56121000000000265</v>
-      </c>
-      <c r="I3" s="3">
-        <f>F3-E3</f>
-        <v>-0.35188999999999737</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="3">
-        <v>23.289580000000001</v>
-      </c>
-      <c r="N3" s="3">
-        <v>23.46311</v>
-      </c>
-      <c r="O3" s="3">
-        <v>23.089919999999999</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3">
-        <f>N3-M3</f>
-        <v>0.17352999999999952</v>
-      </c>
-      <c r="R3" s="3">
-        <f>O3-N3</f>
-        <v>-0.37319000000000102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>32</v>
+        <v>0.1072046</v>
+      </c>
+      <c r="G3">
+        <v>1.9761000000000002E-3</v>
+      </c>
+      <c r="H3">
+        <v>3.475422</v>
+      </c>
+      <c r="I3">
+        <v>9.6336000000000008E-3</v>
+      </c>
+      <c r="J3">
+        <v>9.6336000000000008E-3</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>3.4499799999999997E-2</v>
+      </c>
+      <c r="M3">
+        <v>1.8938E-3</v>
+      </c>
+      <c r="N3">
+        <v>17701.25</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>17720.64</v>
+      </c>
+      <c r="Q3">
+        <v>14682.41</v>
+      </c>
+      <c r="R3">
+        <v>1032.5260000000001</v>
+      </c>
+      <c r="S3">
+        <v>-3009.9090000000001</v>
+      </c>
+      <c r="T3">
+        <v>0.5864142</v>
+      </c>
+      <c r="U3">
+        <v>0.40559899999999999</v>
+      </c>
+      <c r="V3">
+        <v>7.9868000000000005E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>18.88119</v>
+      </c>
+      <c r="C4">
+        <v>0.35710170000000002</v>
       </c>
       <c r="D4">
-        <v>0.76065970000000005</v>
+        <v>0.15899550000000001</v>
       </c>
       <c r="E4">
-        <v>0.73675749999999995</v>
+        <v>0.48390280000000002</v>
       </c>
       <c r="F4">
-        <v>0.72771839999999999</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" ref="H4:I12" si="0">E4-D4</f>
-        <v>-2.3902200000000096E-2</v>
-      </c>
-      <c r="I4" s="3">
+        <v>8.7855100000000005E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.021E-2</v>
+      </c>
+      <c r="H4">
+        <v>3.410704</v>
+      </c>
+      <c r="I4">
+        <v>1.3750500000000001E-2</v>
+      </c>
+      <c r="J4">
+        <v>1.3750500000000001E-2</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>5.6648799999999999E-2</v>
+      </c>
+      <c r="M4">
+        <v>8.3984999999999997E-3</v>
+      </c>
+      <c r="N4">
+        <v>17771</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>17884.09</v>
+      </c>
+      <c r="Q4">
+        <v>15617.81</v>
+      </c>
+      <c r="R4">
+        <v>1100.3040000000001</v>
+      </c>
+      <c r="S4">
+        <v>-4390.9530000000004</v>
+      </c>
+      <c r="T4">
+        <v>0.42651299999999998</v>
+      </c>
+      <c r="U4">
+        <v>0.53750509999999996</v>
+      </c>
+      <c r="V4">
+        <v>3.5981899999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A13" si="0">A4+1</f>
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>23.55076</v>
+      </c>
+      <c r="C5">
+        <v>0.52350759999999996</v>
+      </c>
+      <c r="D5">
+        <v>0.1104981</v>
+      </c>
+      <c r="E5">
+        <v>0.36599419999999999</v>
+      </c>
+      <c r="F5">
+        <v>6.5706100000000003E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.86908E-2</v>
+      </c>
+      <c r="H5">
+        <v>3.3524910000000001</v>
+      </c>
+      <c r="I5">
+        <v>1.8032099999999999E-2</v>
+      </c>
+      <c r="J5">
+        <v>1.8032099999999999E-2</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>8.0444600000000005E-2</v>
+      </c>
+      <c r="M5">
+        <v>1.50679E-2</v>
+      </c>
+      <c r="N5">
+        <v>15091.37</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>15292.9</v>
+      </c>
+      <c r="Q5">
+        <v>16693.080000000002</v>
+      </c>
+      <c r="R5">
+        <v>1279.1110000000001</v>
+      </c>
+      <c r="S5">
+        <v>-2332.9499999999998</v>
+      </c>
+      <c r="T5">
+        <v>0.30399340000000002</v>
+      </c>
+      <c r="U5">
+        <v>0.60691640000000002</v>
+      </c>
+      <c r="V5">
+        <v>8.9090199999999994E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
         <f t="shared" si="0"/>
-        <v>-9.0390999999999666E-3</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0.75795860000000004</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0.7593858</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0.74977079999999996</v>
-      </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="2">
-        <f t="shared" ref="Q4:Q12" si="1">N4-M4</f>
-        <v>1.4271999999999618E-3</v>
-      </c>
-      <c r="R4" s="3">
-        <f t="shared" ref="R4:R12" si="2">O4-N4</f>
-        <v>-9.6150000000000402E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5">
-        <v>0.1739039</v>
-      </c>
-      <c r="E5">
-        <v>0.1735748</v>
-      </c>
-      <c r="F5">
-        <v>0.17640040000000001</v>
-      </c>
-      <c r="H5" s="3">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>25.111160000000002</v>
+      </c>
+      <c r="C6">
+        <v>0.64775629999999995</v>
+      </c>
+      <c r="D6">
+        <v>8.6373000000000005E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.26587070000000002</v>
+      </c>
+      <c r="F6">
+        <v>5.0885100000000003E-2</v>
+      </c>
+      <c r="G6">
+        <v>3.2688300000000003E-2</v>
+      </c>
+      <c r="H6">
+        <v>3.3194729999999999</v>
+      </c>
+      <c r="I6">
+        <v>2.2478399999999999E-2</v>
+      </c>
+      <c r="J6">
+        <v>2.2478399999999999E-2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>9.0901599999999999E-2</v>
+      </c>
+      <c r="M6">
+        <v>2.7418700000000001E-2</v>
+      </c>
+      <c r="N6">
+        <v>15646.72</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>16007.04</v>
+      </c>
+      <c r="Q6">
+        <v>17606.04</v>
+      </c>
+      <c r="R6">
+        <v>1407.0809999999999</v>
+      </c>
+      <c r="S6">
+        <v>25.67923</v>
+      </c>
+      <c r="T6">
+        <v>0.21432689999999999</v>
+      </c>
+      <c r="U6">
+        <v>0.62149030000000005</v>
+      </c>
+      <c r="V6">
+        <v>0.16418279999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
         <f t="shared" si="0"/>
-        <v>-3.2909999999999884E-4</v>
-      </c>
-      <c r="I5" s="3">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>20.840019999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.67015230000000003</v>
+      </c>
+      <c r="D7">
+        <v>0.14491560000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.18493209999999999</v>
+      </c>
+      <c r="F7">
+        <v>4.8579700000000003E-2</v>
+      </c>
+      <c r="G7">
+        <v>4.6850599999999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>3.2941950000000002</v>
+      </c>
+      <c r="I7">
+        <v>2.1737300000000001E-2</v>
+      </c>
+      <c r="J7">
+        <v>2.1737300000000001E-2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>9.5018500000000006E-2</v>
+      </c>
+      <c r="M7">
+        <v>3.9440099999999999E-2</v>
+      </c>
+      <c r="N7">
+        <v>16461.03</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>17003.400000000001</v>
+      </c>
+      <c r="Q7">
+        <v>17120.240000000002</v>
+      </c>
+      <c r="R7">
+        <v>1292.4929999999999</v>
+      </c>
+      <c r="S7">
+        <v>2142.4319999999998</v>
+      </c>
+      <c r="T7">
+        <v>0.1480445</v>
+      </c>
+      <c r="U7">
+        <v>0.60823380000000005</v>
+      </c>
+      <c r="V7">
+        <v>0.24372170000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
         <f t="shared" si="0"/>
-        <v>2.8256000000000114E-3</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0.17382210000000001</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0.17506179999999999</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0.17768690000000001</v>
-      </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3">
-        <f t="shared" si="1"/>
-        <v>1.2396999999999825E-3</v>
-      </c>
-      <c r="R5" s="3">
-        <f t="shared" si="2"/>
-        <v>2.6251000000000191E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>3.2975299999999999E-2</v>
-      </c>
-      <c r="E6">
-        <v>3.8560700000000003E-2</v>
-      </c>
-      <c r="F6">
-        <v>3.7917600000000003E-2</v>
-      </c>
-      <c r="H6" s="3">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>17.112310000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.61021000000000003</v>
+      </c>
+      <c r="D8">
+        <v>0.25755450000000002</v>
+      </c>
+      <c r="E8">
+        <v>0.13223550000000001</v>
+      </c>
+      <c r="F8">
+        <v>4.6027199999999997E-2</v>
+      </c>
+      <c r="G8">
+        <v>5.9530699999999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>3.27007</v>
+      </c>
+      <c r="I8">
+        <v>2.5277899999999999E-2</v>
+      </c>
+      <c r="J8">
+        <v>2.5277899999999999E-2</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>9.57596E-2</v>
+      </c>
+      <c r="M8">
+        <v>5.0061799999999997E-2</v>
+      </c>
+      <c r="N8">
+        <v>17331.8</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>18035.98</v>
+      </c>
+      <c r="Q8">
+        <v>15885.31</v>
+      </c>
+      <c r="R8">
+        <v>1114.047</v>
+      </c>
+      <c r="S8">
+        <v>2338.7350000000001</v>
+      </c>
+      <c r="T8">
+        <v>0.1044051</v>
+      </c>
+      <c r="U8">
+        <v>0.58476740000000005</v>
+      </c>
+      <c r="V8">
+        <v>0.31082749999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f t="shared" si="0"/>
-        <v>5.5854000000000043E-3</v>
-      </c>
-      <c r="I6" s="3">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>19.518899999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.70201729999999996</v>
+      </c>
+      <c r="D9">
+        <v>0.2098806</v>
+      </c>
+      <c r="E9">
+        <v>8.8102100000000003E-2</v>
+      </c>
+      <c r="F9">
+        <v>5.8707299999999997E-2</v>
+      </c>
+      <c r="G9">
+        <v>7.5669E-2</v>
+      </c>
+      <c r="H9">
+        <v>3.2275830000000001</v>
+      </c>
+      <c r="I9">
+        <v>3.5405499999999999E-2</v>
+      </c>
+      <c r="J9">
+        <v>3.5405499999999999E-2</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>9.99588E-2</v>
+      </c>
+      <c r="M9">
+        <v>6.4306299999999997E-2</v>
+      </c>
+      <c r="N9">
+        <v>17958.27</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>18886.57</v>
+      </c>
+      <c r="Q9">
+        <v>18062.990000000002</v>
+      </c>
+      <c r="R9">
+        <v>1442.905</v>
+      </c>
+      <c r="S9">
+        <v>4603.9350000000004</v>
+      </c>
+      <c r="T9">
+        <v>7.3116500000000001E-2</v>
+      </c>
+      <c r="U9">
+        <v>0.56401809999999997</v>
+      </c>
+      <c r="V9">
+        <v>0.3628654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f t="shared" si="0"/>
-        <v>-6.4310000000000062E-4</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1.8915010000000001</v>
-      </c>
-      <c r="F7">
-        <v>1.893581</v>
-      </c>
-      <c r="H7" s="3">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>18.326879999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.69263070000000004</v>
+      </c>
+      <c r="D10">
+        <v>0.24676819999999999</v>
+      </c>
+      <c r="E10">
+        <v>6.0601099999999998E-2</v>
+      </c>
+      <c r="F10">
+        <v>4.8085599999999999E-2</v>
+      </c>
+      <c r="G10">
+        <v>9.72417E-2</v>
+      </c>
+      <c r="H10">
+        <v>3.2153969999999998</v>
+      </c>
+      <c r="I10">
+        <v>3.4993799999999999E-2</v>
+      </c>
+      <c r="J10">
+        <v>3.4993799999999999E-2</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0.1067106</v>
+      </c>
+      <c r="M10">
+        <v>8.3573499999999995E-2</v>
+      </c>
+      <c r="N10">
+        <v>18662.509999999998</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>19911.02</v>
+      </c>
+      <c r="Q10">
+        <v>17983.52</v>
+      </c>
+      <c r="R10">
+        <v>1437.347</v>
+      </c>
+      <c r="S10">
+        <v>7027.4250000000002</v>
+      </c>
+      <c r="T10">
+        <v>5.3602299999999999E-2</v>
+      </c>
+      <c r="U10">
+        <v>0.54952659999999998</v>
+      </c>
+      <c r="V10">
+        <v>0.39687109999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
         <f t="shared" si="0"/>
-        <v>1.8915010000000001</v>
-      </c>
-      <c r="I7" s="3">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>18.25854</v>
+      </c>
+      <c r="C11">
+        <v>0.69790039999999998</v>
+      </c>
+      <c r="D11">
+        <v>0.2621655</v>
+      </c>
+      <c r="E11">
+        <v>3.99341E-2</v>
+      </c>
+      <c r="F11">
+        <v>4.9073699999999998E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.1170852</v>
+      </c>
+      <c r="H11">
+        <v>3.1904490000000001</v>
+      </c>
+      <c r="I11">
+        <v>4.0839899999999998E-2</v>
+      </c>
+      <c r="J11">
+        <v>4.0839899999999998E-2</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0.1143681</v>
+      </c>
+      <c r="M11">
+        <v>0.1016879</v>
+      </c>
+      <c r="N11">
+        <v>19644.59</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>21159.119999999999</v>
+      </c>
+      <c r="Q11">
+        <v>18392.439999999999</v>
+      </c>
+      <c r="R11">
+        <v>1507.7660000000001</v>
+      </c>
+      <c r="S11">
+        <v>6663.94</v>
+      </c>
+      <c r="T11">
+        <v>4.0757500000000002E-2</v>
+      </c>
+      <c r="U11">
+        <v>0.53684639999999995</v>
+      </c>
+      <c r="V11">
+        <v>0.42239599999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
         <f t="shared" si="0"/>
-        <v>2.0799999999998597E-3</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3">
-        <v>1.782767</v>
-      </c>
-      <c r="O7" s="3">
-        <v>1.7798609999999999</v>
-      </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3">
-        <f t="shared" si="1"/>
-        <v>1.782767</v>
-      </c>
-      <c r="R7" s="3">
-        <f t="shared" si="2"/>
-        <v>-2.9060000000000752E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>20.96097</v>
+      </c>
+      <c r="C12">
+        <v>0.78830789999999995</v>
+      </c>
+      <c r="D12">
+        <v>0.18089749999999999</v>
+      </c>
+      <c r="E12">
+        <v>3.0794599999999998E-2</v>
+      </c>
+      <c r="F12">
+        <v>5.0226399999999997E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.14013999999999999</v>
+      </c>
+      <c r="H12">
+        <v>3.1890489999999998</v>
+      </c>
+      <c r="I12">
+        <v>4.0922199999999999E-2</v>
+      </c>
+      <c r="J12">
+        <v>4.0922199999999999E-2</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0.1174969</v>
+      </c>
+      <c r="M12">
+        <v>0.1227666</v>
+      </c>
+      <c r="N12">
+        <v>20059.34</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>21910.85</v>
+      </c>
+      <c r="Q12">
+        <v>19882.71</v>
+      </c>
+      <c r="R12">
+        <v>1762.289</v>
+      </c>
+      <c r="S12">
+        <v>9589.6180000000004</v>
+      </c>
+      <c r="T12">
+        <v>3.3182400000000001E-2</v>
+      </c>
+      <c r="U12">
+        <v>0.52803619999999996</v>
+      </c>
+      <c r="V12">
+        <v>0.43878139999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>9.3740000000000002E-4</v>
-      </c>
-      <c r="F9">
-        <v>2.4965999999999999E-3</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
-        <v>9.3740000000000002E-4</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5591999999999997E-3</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="3">
-        <v>0</v>
-      </c>
-      <c r="N9" s="3">
-        <v>9.7499999999999996E-4</v>
-      </c>
-      <c r="O9" s="3">
-        <v>2.5950000000000001E-3</v>
-      </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3">
-        <f t="shared" si="1"/>
-        <v>9.7499999999999996E-4</v>
-      </c>
-      <c r="R9" s="3">
-        <f t="shared" si="2"/>
-        <v>1.6200000000000001E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>20629.310000000001</v>
-      </c>
-      <c r="E10">
-        <v>20178.46</v>
-      </c>
-      <c r="F10">
-        <v>20157.830000000002</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
-        <v>-450.85000000000218</v>
-      </c>
-      <c r="I10" s="3">
-        <f t="shared" si="0"/>
-        <v>-20.629999999997381</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10" s="3">
-        <v>20702.849999999999</v>
-      </c>
-      <c r="N10" s="3">
-        <v>20497</v>
-      </c>
-      <c r="O10" s="3">
-        <v>20465.13</v>
-      </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3">
-        <f t="shared" si="1"/>
-        <v>-205.84999999999854</v>
-      </c>
-      <c r="R10" s="3">
-        <f t="shared" si="2"/>
-        <v>-31.869999999998981</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>1726.18</v>
-      </c>
-      <c r="E11">
-        <v>1683.373</v>
-      </c>
-      <c r="F11">
-        <v>1676.4490000000001</v>
-      </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>-42.807000000000016</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" si="0"/>
-        <v>-6.9239999999999782</v>
-      </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="3">
-        <v>1736.2550000000001</v>
-      </c>
-      <c r="N11" s="3">
-        <v>1722.9960000000001</v>
-      </c>
-      <c r="O11" s="3">
-        <v>1714.568</v>
-      </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3">
-        <f t="shared" si="1"/>
-        <v>-13.259000000000015</v>
-      </c>
-      <c r="R11" s="3">
-        <f t="shared" si="2"/>
-        <v>-8.428000000000111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12">
-        <v>8530.8520000000008</v>
-      </c>
-      <c r="E12">
-        <v>7499.4530000000004</v>
-      </c>
-      <c r="F12">
-        <v>7709.9210000000003</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="0"/>
-        <v>-1031.3990000000003</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" si="0"/>
-        <v>210.46799999999985</v>
-      </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="3">
-        <v>8963.5879999999997</v>
-      </c>
-      <c r="N12" s="3">
-        <v>8360.3950000000004</v>
-      </c>
-      <c r="O12" s="3">
-        <v>8543.64</v>
-      </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3">
-        <f t="shared" si="1"/>
-        <v>-603.1929999999993</v>
-      </c>
-      <c r="R12" s="3">
-        <f t="shared" si="2"/>
-        <v>183.24499999999898</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15">
-        <v>23.289580000000001</v>
-      </c>
-      <c r="E15" s="3">
-        <v>23.211069999999999</v>
-      </c>
-      <c r="F15">
-        <v>23.16339</v>
-      </c>
-      <c r="H15" s="3">
-        <f>E15-D15</f>
-        <v>-7.8510000000001412E-2</v>
-      </c>
-      <c r="I15" s="3">
-        <f>F15-E15</f>
-        <v>-4.7679999999999723E-2</v>
-      </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16">
-        <v>0.75795860000000004</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.74353849999999999</v>
-      </c>
-      <c r="F16">
-        <v>0.74078540000000004</v>
-      </c>
-      <c r="H16" s="3">
-        <f>E16-D16</f>
-        <v>-1.4420100000000047E-2</v>
-      </c>
-      <c r="I16" s="3">
-        <f>F16-E16</f>
-        <v>-2.7530999999999528E-3</v>
-      </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17">
-        <v>0.17382210000000001</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0.1644351</v>
-      </c>
-      <c r="F17">
-        <v>0.1668789</v>
-      </c>
-      <c r="H17" s="3">
-        <f t="shared" ref="H16:H24" si="3">E17-D17</f>
-        <v>-9.3870000000000064E-3</v>
-      </c>
-      <c r="I17" s="3">
-        <f t="shared" ref="I16:I24" si="4">F17-E17</f>
-        <v>2.443799999999996E-3</v>
-      </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>5.1190000000000003E-4</v>
-      </c>
-      <c r="F21">
-        <v>1.5254999999999999E-3</v>
-      </c>
-      <c r="H21" s="3">
-        <f t="shared" si="3"/>
-        <v>5.1190000000000003E-4</v>
-      </c>
-      <c r="I21" s="3">
-        <f t="shared" si="4"/>
-        <v>1.0135999999999999E-3</v>
-      </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22">
-        <v>20702.849999999999</v>
-      </c>
-      <c r="E22" s="3">
-        <v>20400.830000000002</v>
-      </c>
-      <c r="F22">
-        <v>20384.36</v>
-      </c>
-      <c r="H22" s="3">
-        <f t="shared" si="3"/>
-        <v>-302.0199999999968</v>
-      </c>
-      <c r="I22" s="3">
-        <f t="shared" si="4"/>
-        <v>-16.470000000001164</v>
-      </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23">
-        <v>1736.2550000000001</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1710.8050000000001</v>
-      </c>
-      <c r="F23">
-        <v>1711.6479999999999</v>
-      </c>
-      <c r="H23" s="3">
-        <f t="shared" si="3"/>
-        <v>-25.450000000000045</v>
-      </c>
-      <c r="I23" s="3">
-        <f t="shared" si="4"/>
-        <v>0.8429999999998472</v>
-      </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24">
-        <v>8963.5879999999997</v>
-      </c>
-      <c r="E24" s="3">
-        <v>7221.03</v>
-      </c>
-      <c r="F24">
-        <v>7315.268</v>
-      </c>
-      <c r="H24" s="3">
-        <f t="shared" si="3"/>
-        <v>-1742.558</v>
-      </c>
-      <c r="I24" s="3">
-        <f t="shared" si="4"/>
-        <v>94.238000000000284</v>
-      </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27">
-        <v>25.556719999999999</v>
-      </c>
-      <c r="E27">
-        <v>25.465769999999999</v>
-      </c>
-      <c r="F27">
-        <v>25.08727</v>
-      </c>
-      <c r="H27" s="3">
-        <f>E27-D27</f>
-        <v>-9.094999999999942E-2</v>
-      </c>
-      <c r="I27" s="3">
-        <f>F27-E27</f>
-        <v>-0.37849999999999895</v>
-      </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M27" s="3">
-        <v>26.119430000000001</v>
-      </c>
-      <c r="N27" s="3">
-        <v>26.14228</v>
-      </c>
-      <c r="O27" s="3">
-        <v>25.739789999999999</v>
-      </c>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3">
-        <f>N27-M27</f>
-        <v>2.2849999999998261E-2</v>
-      </c>
-      <c r="R27" s="3">
-        <f>O27-N27</f>
-        <v>-0.40249000000000024</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28">
-        <v>0.94943279999999997</v>
-      </c>
-      <c r="E28">
-        <v>0.93973530000000005</v>
-      </c>
-      <c r="F28">
-        <v>0.92514850000000004</v>
-      </c>
-      <c r="H28" s="3">
-        <f t="shared" ref="H28:H36" si="5">E28-D28</f>
-        <v>-9.6974999999999145E-3</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" ref="I28:I36" si="6">F28-E28</f>
-        <v>-1.4586800000000011E-2</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M28" s="3">
-        <v>0.98987539999999996</v>
-      </c>
-      <c r="N28" s="3">
-        <v>0.98338999999999999</v>
-      </c>
-      <c r="O28" s="3">
-        <v>0.9678213</v>
-      </c>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3">
-        <f t="shared" ref="Q28:Q36" si="7">N28-M28</f>
-        <v>-6.4853999999999745E-3</v>
-      </c>
-      <c r="R28" s="2">
-        <f t="shared" ref="R28:R36" si="8">O28-N28</f>
-        <v>-1.5568699999999991E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29">
-        <v>0.42871150000000002</v>
-      </c>
-      <c r="E29">
-        <v>0.43559870000000001</v>
-      </c>
-      <c r="F29">
-        <v>0.43512790000000001</v>
-      </c>
-      <c r="H29" s="3">
-        <f t="shared" si="5"/>
-        <v>6.8871999999999822E-3</v>
-      </c>
-      <c r="I29" s="3">
-        <f t="shared" si="6"/>
-        <v>-4.7079999999999345E-4</v>
-      </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M29" s="3">
-        <v>0.48780400000000002</v>
-      </c>
-      <c r="N29" s="3">
-        <v>0.4944905</v>
-      </c>
-      <c r="O29" s="3">
-        <v>0.49488589999999999</v>
-      </c>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3">
-        <f t="shared" si="7"/>
-        <v>6.6864999999999841E-3</v>
-      </c>
-      <c r="R29" s="3">
-        <f t="shared" si="8"/>
-        <v>3.953999999999902E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30">
-        <v>3.3427600000000002E-2</v>
-      </c>
-      <c r="E30">
-        <v>3.8157999999999997E-2</v>
-      </c>
-      <c r="F30">
-        <v>3.5815300000000001E-2</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" si="5"/>
-        <v>4.7303999999999957E-3</v>
-      </c>
-      <c r="I30" s="3">
-        <f t="shared" si="6"/>
-        <v>-2.3426999999999962E-3</v>
-      </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M30" s="3">
-        <v>3.29717E-2</v>
-      </c>
-      <c r="N30" s="3">
-        <v>3.6439600000000003E-2</v>
-      </c>
-      <c r="O30" s="3">
-        <v>3.5042400000000001E-2</v>
-      </c>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3">
-        <f t="shared" si="7"/>
-        <v>3.4679000000000029E-3</v>
-      </c>
-      <c r="R30" s="3">
-        <f t="shared" si="8"/>
-        <v>-1.3972000000000012E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>2.3181419999999999</v>
-      </c>
-      <c r="F31">
-        <v>2.2793049999999999</v>
-      </c>
-      <c r="H31" s="3">
-        <f t="shared" si="5"/>
-        <v>2.3181419999999999</v>
-      </c>
-      <c r="I31" s="3">
-        <f t="shared" si="6"/>
-        <v>-3.883700000000001E-2</v>
-      </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M31" s="3">
-        <v>0</v>
-      </c>
-      <c r="N31" s="3">
-        <v>2.3061370000000001</v>
-      </c>
-      <c r="O31" s="3">
-        <v>2.3139780000000001</v>
-      </c>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3">
-        <f t="shared" si="7"/>
-        <v>2.3061370000000001</v>
-      </c>
-      <c r="R31" s="3">
-        <f t="shared" si="8"/>
-        <v>7.8409999999999869E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>15.191789999999999</v>
-      </c>
-      <c r="F32">
-        <v>14.84299</v>
-      </c>
-      <c r="H32" s="2">
-        <f t="shared" si="5"/>
-        <v>15.191789999999999</v>
-      </c>
-      <c r="I32" s="2">
-        <f t="shared" si="6"/>
-        <v>-0.34879999999999889</v>
-      </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M32" s="3">
-        <v>0</v>
-      </c>
-      <c r="N32" s="3">
-        <v>19.099209999999999</v>
-      </c>
-      <c r="O32" s="3">
-        <v>18.708089999999999</v>
-      </c>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="2">
-        <f t="shared" si="7"/>
-        <v>19.099209999999999</v>
-      </c>
-      <c r="R32" s="2">
-        <f t="shared" si="8"/>
-        <v>-0.3911200000000008</v>
-      </c>
-    </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>5.4127000000000003E-3</v>
-      </c>
-      <c r="F33">
-        <v>8.0322999999999992E-3</v>
-      </c>
-      <c r="H33" s="3">
-        <f t="shared" si="5"/>
-        <v>5.4127000000000003E-3</v>
-      </c>
-      <c r="I33" s="3">
-        <f t="shared" si="6"/>
-        <v>2.6195999999999988E-3</v>
-      </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M33" s="3">
-        <v>0</v>
-      </c>
-      <c r="N33" s="3">
-        <v>8.4779999999999994E-3</v>
-      </c>
-      <c r="O33" s="3">
-        <v>1.0044600000000001E-2</v>
-      </c>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3">
-        <f t="shared" si="7"/>
-        <v>8.4779999999999994E-3</v>
-      </c>
-      <c r="R33" s="3">
-        <f t="shared" si="8"/>
-        <v>1.5666000000000013E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34">
-        <v>27854.21</v>
-      </c>
-      <c r="E34">
-        <v>27679.94</v>
-      </c>
-      <c r="F34">
-        <v>27429.67</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="5"/>
-        <v>-174.27000000000044</v>
-      </c>
-      <c r="I34" s="3">
-        <f t="shared" si="6"/>
-        <v>-250.27000000000044</v>
-      </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M34" s="3">
-        <v>29122.15</v>
-      </c>
-      <c r="N34" s="3">
-        <v>28938.73</v>
-      </c>
-      <c r="O34" s="3">
-        <v>28678.959999999999</v>
-      </c>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3">
-        <f t="shared" si="7"/>
-        <v>-183.42000000000189</v>
-      </c>
-      <c r="R34" s="3">
-        <f t="shared" si="8"/>
-        <v>-259.77000000000044</v>
-      </c>
-    </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35">
-        <v>2588.7190000000001</v>
-      </c>
-      <c r="E35">
-        <v>2621.9110000000001</v>
-      </c>
-      <c r="F35">
-        <v>2596.9520000000002</v>
-      </c>
-      <c r="H35" s="3">
-        <f t="shared" si="5"/>
-        <v>33.192000000000007</v>
-      </c>
-      <c r="I35" s="3">
-        <f t="shared" si="6"/>
-        <v>-24.958999999999833</v>
-      </c>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M35" s="3">
-        <v>2697.6509999999998</v>
-      </c>
-      <c r="N35" s="3">
-        <v>2753.8330000000001</v>
-      </c>
-      <c r="O35" s="3">
-        <v>2722.4279999999999</v>
-      </c>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3">
-        <f t="shared" si="7"/>
-        <v>56.182000000000244</v>
-      </c>
-      <c r="R35" s="3">
-        <f t="shared" si="8"/>
-        <v>-31.4050000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36">
-        <v>47973.58</v>
-      </c>
-      <c r="E36">
-        <v>52272.959999999999</v>
-      </c>
-      <c r="F36">
-        <v>50670.89</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" si="5"/>
-        <v>4299.3799999999974</v>
-      </c>
-      <c r="I36" s="2">
-        <f t="shared" si="6"/>
-        <v>-1602.0699999999997</v>
-      </c>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M36" s="3">
-        <v>54872.55</v>
-      </c>
-      <c r="N36" s="3">
-        <v>60766.74</v>
-      </c>
-      <c r="O36" s="3">
-        <v>57252.91</v>
-      </c>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="2">
-        <f t="shared" si="7"/>
-        <v>5894.1899999999951</v>
-      </c>
-      <c r="R36" s="2">
-        <f t="shared" si="8"/>
-        <v>-3513.8299999999945</v>
-      </c>
-    </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-    </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>47</v>
-      </c>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-    </row>
-    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39">
-        <v>26.127359999999999</v>
-      </c>
-      <c r="E39">
-        <v>26.602460000000001</v>
-      </c>
-      <c r="F39">
-        <v>26.211200000000002</v>
-      </c>
-      <c r="H39" s="3">
-        <f>E39-D39</f>
-        <v>0.47510000000000119</v>
-      </c>
-      <c r="I39" s="3">
-        <f>F39-E39</f>
-        <v>-0.39125999999999905</v>
-      </c>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M39" s="3">
-        <v>26.127359999999999</v>
-      </c>
-      <c r="N39" s="3">
-        <v>26.256</v>
-      </c>
-      <c r="O39" s="3">
-        <v>26.29702</v>
-      </c>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3">
-        <f>N39-M39</f>
-        <v>0.12864000000000075</v>
-      </c>
-      <c r="R39" s="3">
-        <f>O39-N39</f>
-        <v>4.1019999999999612E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40">
-        <v>0.98915379999999997</v>
-      </c>
-      <c r="E40">
-        <v>0.99948930000000002</v>
-      </c>
-      <c r="F40">
-        <v>0.98453550000000001</v>
-      </c>
-      <c r="H40" s="2">
-        <f t="shared" ref="H40:H48" si="9">E40-D40</f>
-        <v>1.0335500000000053E-2</v>
-      </c>
-      <c r="I40" s="2">
-        <f t="shared" ref="I40:I48" si="10">F40-E40</f>
-        <v>-1.4953800000000017E-2</v>
-      </c>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M40" s="3">
-        <v>0.98915379999999997</v>
-      </c>
-      <c r="N40" s="3">
-        <v>0.98323130000000003</v>
-      </c>
-      <c r="O40" s="3">
-        <v>0.98133300000000001</v>
-      </c>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3">
-        <f t="shared" ref="Q40:Q48" si="11">N40-M40</f>
-        <v>-5.9224999999999417E-3</v>
-      </c>
-      <c r="R40" s="3">
-        <f t="shared" ref="R40:R48" si="12">O40-N40</f>
-        <v>-1.8983000000000194E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41">
-        <v>0.48689169999999998</v>
-      </c>
-      <c r="E41">
-        <v>0.49629859999999998</v>
-      </c>
-      <c r="F41">
-        <v>0.49652689999999999</v>
-      </c>
-      <c r="H41" s="3">
-        <f t="shared" si="9"/>
-        <v>9.4068999999999958E-3</v>
-      </c>
-      <c r="I41" s="3">
-        <f t="shared" si="10"/>
-        <v>2.283000000000146E-4</v>
-      </c>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M41" s="3">
-        <v>0.48689169999999998</v>
-      </c>
-      <c r="N41" s="3">
-        <v>0.4766936</v>
-      </c>
-      <c r="O41" s="3">
-        <v>0.47651789999999999</v>
-      </c>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3">
-        <f t="shared" si="11"/>
-        <v>-1.0198099999999988E-2</v>
-      </c>
-      <c r="R41" s="3">
-        <f t="shared" si="12"/>
-        <v>-1.7570000000000086E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="H42" s="3">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I42" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M42" s="3">
-        <v>0</v>
-      </c>
-      <c r="N42" s="3">
-        <v>0</v>
-      </c>
-      <c r="O42" s="3">
-        <v>0</v>
-      </c>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="R42" s="3">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>2.0762830000000001</v>
-      </c>
-      <c r="F43">
-        <v>2.0704539999999998</v>
-      </c>
-      <c r="H43" s="3">
-        <f t="shared" si="9"/>
-        <v>2.0762830000000001</v>
-      </c>
-      <c r="I43" s="3">
-        <f t="shared" si="10"/>
-        <v>-5.8290000000003062E-3</v>
-      </c>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M43" s="3">
-        <v>0</v>
-      </c>
-      <c r="N43" s="3">
-        <v>0</v>
-      </c>
-      <c r="O43" s="3">
-        <v>0</v>
-      </c>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="R43" s="3">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>19.458549999999999</v>
-      </c>
-      <c r="F44">
-        <v>19.086569999999998</v>
-      </c>
-      <c r="H44" s="2">
-        <f t="shared" si="9"/>
-        <v>19.458549999999999</v>
-      </c>
-      <c r="I44" s="2">
-        <f t="shared" si="10"/>
-        <v>-0.37198000000000064</v>
-      </c>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M44" s="3">
-        <v>0</v>
-      </c>
-      <c r="N44" s="3">
-        <v>19.483309999999999</v>
-      </c>
-      <c r="O44" s="3">
-        <v>19.227930000000001</v>
-      </c>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="2">
-        <f t="shared" si="11"/>
-        <v>19.483309999999999</v>
-      </c>
-      <c r="R44" s="2">
-        <f t="shared" si="12"/>
-        <v>-0.25537999999999883</v>
-      </c>
-    </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>7.7397999999999998E-3</v>
-      </c>
-      <c r="F45">
-        <v>9.8200000000000006E-3</v>
-      </c>
-      <c r="H45" s="3">
-        <f t="shared" si="9"/>
-        <v>7.7397999999999998E-3</v>
-      </c>
-      <c r="I45" s="3">
-        <f t="shared" si="10"/>
-        <v>2.0802000000000008E-3</v>
-      </c>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M45" s="3">
-        <v>0</v>
-      </c>
-      <c r="N45" s="3">
-        <v>3.2724E-3</v>
-      </c>
-      <c r="O45" s="3">
-        <v>4.1558999999999997E-3</v>
-      </c>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3">
-        <f t="shared" si="11"/>
-        <v>3.2724E-3</v>
-      </c>
-      <c r="R45" s="3">
-        <f t="shared" si="12"/>
-        <v>8.8349999999999974E-4</v>
-      </c>
-    </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46">
-        <v>29181.14</v>
-      </c>
-      <c r="E46">
-        <v>29042.12</v>
-      </c>
-      <c r="F46">
-        <v>28788.98</v>
-      </c>
-      <c r="H46" s="3">
-        <f t="shared" si="9"/>
-        <v>-139.02000000000044</v>
-      </c>
-      <c r="I46" s="3">
-        <f t="shared" si="10"/>
-        <v>-253.13999999999942</v>
-      </c>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M46" s="3">
-        <v>29181.14</v>
-      </c>
-      <c r="N46" s="3">
-        <v>28640.73</v>
-      </c>
-      <c r="O46" s="3">
-        <v>28399.31</v>
-      </c>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3">
-        <f t="shared" si="11"/>
-        <v>-540.40999999999985</v>
-      </c>
-      <c r="R46" s="3">
-        <f t="shared" si="12"/>
-        <v>-241.41999999999825</v>
-      </c>
-    </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47">
-        <v>2710.1010000000001</v>
-      </c>
-      <c r="E47">
-        <v>2775.0010000000002</v>
-      </c>
-      <c r="F47">
-        <v>2743.605</v>
-      </c>
-      <c r="H47" s="3">
-        <f t="shared" si="9"/>
-        <v>64.900000000000091</v>
-      </c>
-      <c r="I47" s="3">
-        <f t="shared" si="10"/>
-        <v>-31.396000000000186</v>
-      </c>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M47" s="3">
-        <v>2710.1010000000001</v>
-      </c>
-      <c r="N47" s="3">
-        <v>2725.134</v>
-      </c>
-      <c r="O47" s="3">
-        <v>2704.8589999999999</v>
-      </c>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3">
-        <f t="shared" si="11"/>
-        <v>15.032999999999902</v>
-      </c>
-      <c r="R47" s="3">
-        <f t="shared" si="12"/>
-        <v>-20.275000000000091</v>
-      </c>
-    </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48">
-        <v>55724.94</v>
-      </c>
-      <c r="E48">
-        <v>61859.99</v>
-      </c>
-      <c r="F48">
-        <v>58063.76</v>
-      </c>
-      <c r="H48" s="2">
-        <f t="shared" si="9"/>
-        <v>6135.0499999999956</v>
-      </c>
-      <c r="I48" s="2">
-        <f t="shared" si="10"/>
-        <v>-3796.2299999999959</v>
-      </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M48" s="3">
-        <v>55724.94</v>
-      </c>
-      <c r="N48" s="3">
-        <v>56536.08</v>
-      </c>
-      <c r="O48" s="3">
-        <v>51976.46</v>
-      </c>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3">
-        <f t="shared" si="11"/>
-        <v>811.13999999999942</v>
-      </c>
-      <c r="R48" s="2">
-        <f t="shared" si="12"/>
-        <v>-4559.6200000000026</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C51" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51">
-        <v>33.558050000000001</v>
-      </c>
-      <c r="E51">
-        <v>33.153730000000003</v>
-      </c>
-      <c r="F51">
-        <v>33.176810000000003</v>
-      </c>
-      <c r="H51" s="3">
-        <f>E51-D51</f>
-        <v>-0.40431999999999846</v>
-      </c>
-      <c r="I51" s="3">
-        <f>F51-E51</f>
-        <v>2.3080000000000211E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C52" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52">
-        <v>1.056799</v>
-      </c>
-      <c r="E52">
-        <v>1.0476179999999999</v>
-      </c>
-      <c r="F52">
-        <v>1.0451109999999999</v>
-      </c>
-      <c r="H52" s="3">
-        <f t="shared" ref="H52:H60" si="13">E52-D52</f>
-        <v>-9.1810000000001057E-3</v>
-      </c>
-      <c r="I52" s="3">
-        <f t="shared" ref="I52:I60" si="14">F52-E52</f>
-        <v>-2.507000000000037E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C53" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53">
-        <v>0.79127919999999996</v>
-      </c>
-      <c r="E53">
-        <v>0.77773689999999995</v>
-      </c>
-      <c r="F53">
-        <v>0.7749045</v>
-      </c>
-      <c r="H53" s="3">
-        <f t="shared" si="13"/>
-        <v>-1.3542300000000007E-2</v>
-      </c>
-      <c r="I53" s="3">
-        <f t="shared" si="14"/>
-        <v>-2.8323999999999572E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="H54" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I54" s="3">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="H55" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I55" s="3">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="H56" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I56" s="3">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>2.4298500000000001E-2</v>
-      </c>
-      <c r="F57">
-        <v>1.9785199999999999E-2</v>
-      </c>
-      <c r="H57" s="3">
-        <f t="shared" si="13"/>
-        <v>2.4298500000000001E-2</v>
-      </c>
-      <c r="I57" s="3">
-        <f t="shared" si="14"/>
-        <v>-4.5133000000000013E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58">
-        <v>33554.01</v>
-      </c>
-      <c r="E58">
-        <v>33573.18</v>
-      </c>
-      <c r="F58">
-        <v>33249.33</v>
-      </c>
-      <c r="H58" s="3">
-        <f t="shared" si="13"/>
-        <v>19.169999999998254</v>
-      </c>
-      <c r="I58" s="3">
-        <f t="shared" si="14"/>
-        <v>-323.84999999999854</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D59">
-        <v>3450.2869999999998</v>
-      </c>
-      <c r="E59">
-        <v>3441.9340000000002</v>
-      </c>
-      <c r="F59">
-        <v>3435.7910000000002</v>
-      </c>
-      <c r="H59" s="3">
-        <f t="shared" si="13"/>
-        <v>-8.3529999999996107</v>
-      </c>
-      <c r="I59" s="3">
-        <f t="shared" si="14"/>
-        <v>-6.1430000000000291</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C60" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60">
-        <v>204525.4</v>
-      </c>
-      <c r="E60">
-        <v>203672</v>
-      </c>
-      <c r="F60">
-        <v>200415.6</v>
-      </c>
-      <c r="H60" s="3">
-        <f t="shared" si="13"/>
-        <v>-853.39999999999418</v>
-      </c>
-      <c r="I60" s="3">
-        <f t="shared" si="14"/>
-        <v>-3256.3999999999942</v>
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>13.49905</v>
+      </c>
+      <c r="C13">
+        <v>0.55916010000000005</v>
+      </c>
+      <c r="D13">
+        <v>0.421655</v>
+      </c>
+      <c r="E13">
+        <v>1.9184799999999998E-2</v>
+      </c>
+      <c r="F13">
+        <v>4.2980699999999997E-2</v>
+      </c>
+      <c r="G13">
+        <v>0.16138330000000001</v>
+      </c>
+      <c r="H13">
+        <v>3.1847669999999999</v>
+      </c>
+      <c r="I13">
+        <v>3.8205000000000003E-2</v>
+      </c>
+      <c r="J13">
+        <v>3.8205000000000003E-2</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0.112886</v>
+      </c>
+      <c r="M13">
+        <v>0.1418691</v>
+      </c>
+      <c r="N13">
+        <v>20995.85</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>23133.599999999999</v>
+      </c>
+      <c r="Q13">
+        <v>15333.18</v>
+      </c>
+      <c r="R13">
+        <v>1218.2260000000001</v>
+      </c>
+      <c r="S13">
+        <v>6739.09</v>
+      </c>
+      <c r="T13">
+        <v>2.86538E-2</v>
+      </c>
+      <c r="U13">
+        <v>0.51939069999999998</v>
+      </c>
+      <c r="V13">
+        <v>0.45195550000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2624,850 +1352,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8658D477-A0FD-4579-B4B5-2D0B91304A87}">
-  <dimension ref="A2:V13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>17.83944</v>
-      </c>
-      <c r="C3">
-        <v>0.2153149</v>
-      </c>
-      <c r="D3">
-        <v>0.16747629999999999</v>
-      </c>
-      <c r="E3">
-        <v>0.61720870000000005</v>
-      </c>
-      <c r="F3">
-        <v>0.1072046</v>
-      </c>
-      <c r="G3">
-        <v>1.9761000000000002E-3</v>
-      </c>
-      <c r="H3">
-        <v>3.475422</v>
-      </c>
-      <c r="I3">
-        <v>9.6336000000000008E-3</v>
-      </c>
-      <c r="J3">
-        <v>9.6336000000000008E-3</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>3.4499799999999997E-2</v>
-      </c>
-      <c r="M3">
-        <v>1.8938E-3</v>
-      </c>
-      <c r="N3">
-        <v>17701.25</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>17720.64</v>
-      </c>
-      <c r="Q3">
-        <v>14682.41</v>
-      </c>
-      <c r="R3">
-        <v>1032.5260000000001</v>
-      </c>
-      <c r="S3">
-        <v>-3009.9090000000001</v>
-      </c>
-      <c r="T3">
-        <v>0.5864142</v>
-      </c>
-      <c r="U3">
-        <v>0.40559899999999999</v>
-      </c>
-      <c r="V3">
-        <v>7.9868000000000005E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>A3+1</f>
-        <v>19</v>
-      </c>
-      <c r="B4">
-        <v>18.88119</v>
-      </c>
-      <c r="C4">
-        <v>0.35710170000000002</v>
-      </c>
-      <c r="D4">
-        <v>0.15899550000000001</v>
-      </c>
-      <c r="E4">
-        <v>0.48390280000000002</v>
-      </c>
-      <c r="F4">
-        <v>8.7855100000000005E-2</v>
-      </c>
-      <c r="G4">
-        <v>1.021E-2</v>
-      </c>
-      <c r="H4">
-        <v>3.410704</v>
-      </c>
-      <c r="I4">
-        <v>1.3750500000000001E-2</v>
-      </c>
-      <c r="J4">
-        <v>1.3750500000000001E-2</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>5.6648799999999999E-2</v>
-      </c>
-      <c r="M4">
-        <v>8.3984999999999997E-3</v>
-      </c>
-      <c r="N4">
-        <v>17771</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>17884.09</v>
-      </c>
-      <c r="Q4">
-        <v>15617.81</v>
-      </c>
-      <c r="R4">
-        <v>1100.3040000000001</v>
-      </c>
-      <c r="S4">
-        <v>-4390.9530000000004</v>
-      </c>
-      <c r="T4">
-        <v>0.42651299999999998</v>
-      </c>
-      <c r="U4">
-        <v>0.53750509999999996</v>
-      </c>
-      <c r="V4">
-        <v>3.5981899999999997E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ref="A5:A13" si="0">A4+1</f>
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>23.55076</v>
-      </c>
-      <c r="C5">
-        <v>0.52350759999999996</v>
-      </c>
-      <c r="D5">
-        <v>0.1104981</v>
-      </c>
-      <c r="E5">
-        <v>0.36599419999999999</v>
-      </c>
-      <c r="F5">
-        <v>6.5706100000000003E-2</v>
-      </c>
-      <c r="G5">
-        <v>1.86908E-2</v>
-      </c>
-      <c r="H5">
-        <v>3.3524910000000001</v>
-      </c>
-      <c r="I5">
-        <v>1.8032099999999999E-2</v>
-      </c>
-      <c r="J5">
-        <v>1.8032099999999999E-2</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>8.0444600000000005E-2</v>
-      </c>
-      <c r="M5">
-        <v>1.50679E-2</v>
-      </c>
-      <c r="N5">
-        <v>15091.37</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>15292.9</v>
-      </c>
-      <c r="Q5">
-        <v>16693.080000000002</v>
-      </c>
-      <c r="R5">
-        <v>1279.1110000000001</v>
-      </c>
-      <c r="S5">
-        <v>-2332.9499999999998</v>
-      </c>
-      <c r="T5">
-        <v>0.30399340000000002</v>
-      </c>
-      <c r="U5">
-        <v>0.60691640000000002</v>
-      </c>
-      <c r="V5">
-        <v>8.9090199999999994E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>25.111160000000002</v>
-      </c>
-      <c r="C6">
-        <v>0.64775629999999995</v>
-      </c>
-      <c r="D6">
-        <v>8.6373000000000005E-2</v>
-      </c>
-      <c r="E6">
-        <v>0.26587070000000002</v>
-      </c>
-      <c r="F6">
-        <v>5.0885100000000003E-2</v>
-      </c>
-      <c r="G6">
-        <v>3.2688300000000003E-2</v>
-      </c>
-      <c r="H6">
-        <v>3.3194729999999999</v>
-      </c>
-      <c r="I6">
-        <v>2.2478399999999999E-2</v>
-      </c>
-      <c r="J6">
-        <v>2.2478399999999999E-2</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>9.0901599999999999E-2</v>
-      </c>
-      <c r="M6">
-        <v>2.7418700000000001E-2</v>
-      </c>
-      <c r="N6">
-        <v>15646.72</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>16007.04</v>
-      </c>
-      <c r="Q6">
-        <v>17606.04</v>
-      </c>
-      <c r="R6">
-        <v>1407.0809999999999</v>
-      </c>
-      <c r="S6">
-        <v>25.67923</v>
-      </c>
-      <c r="T6">
-        <v>0.21432689999999999</v>
-      </c>
-      <c r="U6">
-        <v>0.62149030000000005</v>
-      </c>
-      <c r="V6">
-        <v>0.16418279999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>20.840019999999999</v>
-      </c>
-      <c r="C7">
-        <v>0.67015230000000003</v>
-      </c>
-      <c r="D7">
-        <v>0.14491560000000001</v>
-      </c>
-      <c r="E7">
-        <v>0.18493209999999999</v>
-      </c>
-      <c r="F7">
-        <v>4.8579700000000003E-2</v>
-      </c>
-      <c r="G7">
-        <v>4.6850599999999999E-2</v>
-      </c>
-      <c r="H7">
-        <v>3.2941950000000002</v>
-      </c>
-      <c r="I7">
-        <v>2.1737300000000001E-2</v>
-      </c>
-      <c r="J7">
-        <v>2.1737300000000001E-2</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>9.5018500000000006E-2</v>
-      </c>
-      <c r="M7">
-        <v>3.9440099999999999E-2</v>
-      </c>
-      <c r="N7">
-        <v>16461.03</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>17003.400000000001</v>
-      </c>
-      <c r="Q7">
-        <v>17120.240000000002</v>
-      </c>
-      <c r="R7">
-        <v>1292.4929999999999</v>
-      </c>
-      <c r="S7">
-        <v>2142.4319999999998</v>
-      </c>
-      <c r="T7">
-        <v>0.1480445</v>
-      </c>
-      <c r="U7">
-        <v>0.60823380000000005</v>
-      </c>
-      <c r="V7">
-        <v>0.24372170000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>17.112310000000001</v>
-      </c>
-      <c r="C8">
-        <v>0.61021000000000003</v>
-      </c>
-      <c r="D8">
-        <v>0.25755450000000002</v>
-      </c>
-      <c r="E8">
-        <v>0.13223550000000001</v>
-      </c>
-      <c r="F8">
-        <v>4.6027199999999997E-2</v>
-      </c>
-      <c r="G8">
-        <v>5.9530699999999999E-2</v>
-      </c>
-      <c r="H8">
-        <v>3.27007</v>
-      </c>
-      <c r="I8">
-        <v>2.5277899999999999E-2</v>
-      </c>
-      <c r="J8">
-        <v>2.5277899999999999E-2</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>9.57596E-2</v>
-      </c>
-      <c r="M8">
-        <v>5.0061799999999997E-2</v>
-      </c>
-      <c r="N8">
-        <v>17331.8</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>18035.98</v>
-      </c>
-      <c r="Q8">
-        <v>15885.31</v>
-      </c>
-      <c r="R8">
-        <v>1114.047</v>
-      </c>
-      <c r="S8">
-        <v>2338.7350000000001</v>
-      </c>
-      <c r="T8">
-        <v>0.1044051</v>
-      </c>
-      <c r="U8">
-        <v>0.58476740000000005</v>
-      </c>
-      <c r="V8">
-        <v>0.31082749999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>19.518899999999999</v>
-      </c>
-      <c r="C9">
-        <v>0.70201729999999996</v>
-      </c>
-      <c r="D9">
-        <v>0.2098806</v>
-      </c>
-      <c r="E9">
-        <v>8.8102100000000003E-2</v>
-      </c>
-      <c r="F9">
-        <v>5.8707299999999997E-2</v>
-      </c>
-      <c r="G9">
-        <v>7.5669E-2</v>
-      </c>
-      <c r="H9">
-        <v>3.2275830000000001</v>
-      </c>
-      <c r="I9">
-        <v>3.5405499999999999E-2</v>
-      </c>
-      <c r="J9">
-        <v>3.5405499999999999E-2</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>9.99588E-2</v>
-      </c>
-      <c r="M9">
-        <v>6.4306299999999997E-2</v>
-      </c>
-      <c r="N9">
-        <v>17958.27</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>18886.57</v>
-      </c>
-      <c r="Q9">
-        <v>18062.990000000002</v>
-      </c>
-      <c r="R9">
-        <v>1442.905</v>
-      </c>
-      <c r="S9">
-        <v>4603.9350000000004</v>
-      </c>
-      <c r="T9">
-        <v>7.3116500000000001E-2</v>
-      </c>
-      <c r="U9">
-        <v>0.56401809999999997</v>
-      </c>
-      <c r="V9">
-        <v>0.3628654</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B10">
-        <v>18.326879999999999</v>
-      </c>
-      <c r="C10">
-        <v>0.69263070000000004</v>
-      </c>
-      <c r="D10">
-        <v>0.24676819999999999</v>
-      </c>
-      <c r="E10">
-        <v>6.0601099999999998E-2</v>
-      </c>
-      <c r="F10">
-        <v>4.8085599999999999E-2</v>
-      </c>
-      <c r="G10">
-        <v>9.72417E-2</v>
-      </c>
-      <c r="H10">
-        <v>3.2153969999999998</v>
-      </c>
-      <c r="I10">
-        <v>3.4993799999999999E-2</v>
-      </c>
-      <c r="J10">
-        <v>3.4993799999999999E-2</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0.1067106</v>
-      </c>
-      <c r="M10">
-        <v>8.3573499999999995E-2</v>
-      </c>
-      <c r="N10">
-        <v>18662.509999999998</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>19911.02</v>
-      </c>
-      <c r="Q10">
-        <v>17983.52</v>
-      </c>
-      <c r="R10">
-        <v>1437.347</v>
-      </c>
-      <c r="S10">
-        <v>7027.4250000000002</v>
-      </c>
-      <c r="T10">
-        <v>5.3602299999999999E-2</v>
-      </c>
-      <c r="U10">
-        <v>0.54952659999999998</v>
-      </c>
-      <c r="V10">
-        <v>0.39687109999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B11">
-        <v>18.25854</v>
-      </c>
-      <c r="C11">
-        <v>0.69790039999999998</v>
-      </c>
-      <c r="D11">
-        <v>0.2621655</v>
-      </c>
-      <c r="E11">
-        <v>3.99341E-2</v>
-      </c>
-      <c r="F11">
-        <v>4.9073699999999998E-2</v>
-      </c>
-      <c r="G11">
-        <v>0.1170852</v>
-      </c>
-      <c r="H11">
-        <v>3.1904490000000001</v>
-      </c>
-      <c r="I11">
-        <v>4.0839899999999998E-2</v>
-      </c>
-      <c r="J11">
-        <v>4.0839899999999998E-2</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0.1143681</v>
-      </c>
-      <c r="M11">
-        <v>0.1016879</v>
-      </c>
-      <c r="N11">
-        <v>19644.59</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>21159.119999999999</v>
-      </c>
-      <c r="Q11">
-        <v>18392.439999999999</v>
-      </c>
-      <c r="R11">
-        <v>1507.7660000000001</v>
-      </c>
-      <c r="S11">
-        <v>6663.94</v>
-      </c>
-      <c r="T11">
-        <v>4.0757500000000002E-2</v>
-      </c>
-      <c r="U11">
-        <v>0.53684639999999995</v>
-      </c>
-      <c r="V11">
-        <v>0.42239599999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B12">
-        <v>20.96097</v>
-      </c>
-      <c r="C12">
-        <v>0.78830789999999995</v>
-      </c>
-      <c r="D12">
-        <v>0.18089749999999999</v>
-      </c>
-      <c r="E12">
-        <v>3.0794599999999998E-2</v>
-      </c>
-      <c r="F12">
-        <v>5.0226399999999997E-2</v>
-      </c>
-      <c r="G12">
-        <v>0.14013999999999999</v>
-      </c>
-      <c r="H12">
-        <v>3.1890489999999998</v>
-      </c>
-      <c r="I12">
-        <v>4.0922199999999999E-2</v>
-      </c>
-      <c r="J12">
-        <v>4.0922199999999999E-2</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0.1174969</v>
-      </c>
-      <c r="M12">
-        <v>0.1227666</v>
-      </c>
-      <c r="N12">
-        <v>20059.34</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>21910.85</v>
-      </c>
-      <c r="Q12">
-        <v>19882.71</v>
-      </c>
-      <c r="R12">
-        <v>1762.289</v>
-      </c>
-      <c r="S12">
-        <v>9589.6180000000004</v>
-      </c>
-      <c r="T12">
-        <v>3.3182400000000001E-2</v>
-      </c>
-      <c r="U12">
-        <v>0.52803619999999996</v>
-      </c>
-      <c r="V12">
-        <v>0.43878139999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B13">
-        <v>13.49905</v>
-      </c>
-      <c r="C13">
-        <v>0.55916010000000005</v>
-      </c>
-      <c r="D13">
-        <v>0.421655</v>
-      </c>
-      <c r="E13">
-        <v>1.9184799999999998E-2</v>
-      </c>
-      <c r="F13">
-        <v>4.2980699999999997E-2</v>
-      </c>
-      <c r="G13">
-        <v>0.16138330000000001</v>
-      </c>
-      <c r="H13">
-        <v>3.1847669999999999</v>
-      </c>
-      <c r="I13">
-        <v>3.8205000000000003E-2</v>
-      </c>
-      <c r="J13">
-        <v>3.8205000000000003E-2</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0.112886</v>
-      </c>
-      <c r="M13">
-        <v>0.1418691</v>
-      </c>
-      <c r="N13">
-        <v>20995.85</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>23133.599999999999</v>
-      </c>
-      <c r="Q13">
-        <v>15333.18</v>
-      </c>
-      <c r="R13">
-        <v>1218.2260000000001</v>
-      </c>
-      <c r="S13">
-        <v>6739.09</v>
-      </c>
-      <c r="T13">
-        <v>2.86538E-2</v>
-      </c>
-      <c r="U13">
-        <v>0.51939069999999998</v>
-      </c>
-      <c r="V13">
-        <v>0.45195550000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B957CDA-4370-4F60-81CF-A25A00398411}">
   <dimension ref="A2:V13"/>
   <sheetViews>
@@ -4311,7 +2195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A880558E-4514-4D44-996F-A49E3AF6D601}">
   <dimension ref="A2:V13"/>
   <sheetViews>
@@ -5155,7 +3039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68E4EA0-8D54-49A9-ABC6-C424FF8537A1}">
   <dimension ref="A2:V22"/>
   <sheetViews>
@@ -6358,7 +4242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056BE4A6-F579-40E7-8355-0FA3C4ECC0AC}">
   <dimension ref="A2:V15"/>
   <sheetViews>
@@ -7522,7 +5406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A58C0F3-1BB8-4EC8-BF48-2783C76617DE}">
   <dimension ref="A2:V15"/>
   <sheetViews>

</xml_diff>